<commit_message>
löschen von template_path aus gui
</commit_message>
<xml_diff>
--- a/output/3.5._Manufacture_of_energy_efficiency_equipment_for_buildings/DNF_3.5. Manufacture of energy efficiency equipment for buildings.xlsx
+++ b/output/3.5._Manufacture_of_energy_efficiency_equipment_for_buildings/DNF_3.5. Manufacture of energy efficiency equipment for buildings.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,378 +560,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Climate Change Adaptation</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Product | Project</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Climate Change Mitigation</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Climate Change Adaptation</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Product | Project</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>(((((ePBN114211_1=0)&amp;ePBN115002_1&amp;ePBN114210_1)|(((ePBN113603_1=0)|(ePBN113603_1&amp;ePBN113601_1&amp;(ePBN113602_1=0))|(ePBN113603_1&amp;ePBN113601_1&amp;ePBN113602_1&amp;ePBN111305_1&amp;(ePBN113604_1=0))|(ePBN113603_1&amp;ePBN113601_1&amp;ePBN113602_1&amp;ePBN111305_1&amp;ePBN113604_1&amp;ePBN113605_1))&amp;ePBN111303_1)&amp;ePBN114211_1)&amp;(ePBN990109_1=0))|ePBN990109_1)&amp;ePBN110911_1</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>FAILED</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Expected RPAREN but got LITERAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Water</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Project</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Climate Change Mitigation</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Water</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Project</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>((ePBN990111_1|((ePBN990111_1=0)&amp;ePBN992712_1&amp;(ePBN992711_1=0))|((ePBN990111_1=0)&amp;ePBN992712_1&amp;ePBN992711_1&amp;ePBN992708_1&amp;(ePBN992710_1=0))|((ePBN990111_1=0)&amp;ePBN992712_1&amp;ePBN992711_1&amp;ePBN992708_1&amp;ePBN992710_1&amp;ePBN992709_1))&amp;ePBN114211_1)&amp;ePBN110911_1</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Expected RPAREN but got LPAREN</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Circular Economy</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Climate Change Mitigation</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Circular Economy</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>((ePBN990113_1|((ePBN990113_1=0)&amp;ePBN114316_1&amp;ePBN114317_1&amp;ePBN115001_1))&amp;(ePBN114211_1=0))&amp;ePBN110911_1</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>FAILED</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Expected RPAREN but got LPAREN</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>PollutionPrevention and Control</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Product &amp; Project</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Climate Change Mitigation</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>PollutionPrevention and Control</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Product &amp; Project</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>(ePBN990115_1|((ePBN990115_1=0)&amp;ePBN113903_1&amp;(ePBN113904_1=0))|((ePBN990115_1=0)&amp;ePBN113904_1&amp;ePBN113903_1&amp;ePBN113905_1&amp;(ePBN114205_1=0)&amp;ePBN114206_1)|((ePBN990115_1=0)&amp;ePBN113903_1&amp;ePBN113904_1&amp;ePBN113905_1&amp;ePBN114205_1&amp;ePBN113902_1&amp;ePBN114206_1)|((ePBN990115_1=0)&amp;ePBN113903_1&amp;ePBN113904_1&amp;(ePBN113905_1=0)&amp;ePBN113902_1&amp;ePBN114206_1))&amp;ePBN110911_1</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>FAILED</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Expected RPAREN but got LPAREN</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Biodiversity</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Project</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Climate Change Mitigation</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Biodiversity</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Project</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>((ePBN990117_1|((ePBN990117_1=0)&amp;ePBN992713_1&amp;(ePBN992714_1=0))|((ePBN990117_1=0)&amp;ePBN992713_1&amp;ePBN992714_1&amp;ePBN992715_1&amp;(ePBN992717_1=0))|((ePBN990117_1=0)&amp;ePBN992713_1&amp;ePBN992714_1&amp;ePBN992717_1&amp;ePBN992715_1&amp;ePBN992716_1&amp;(ePBN992701_1=0)))&amp;ePBN114211_1)&amp;ePBN110911_1</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>FAILED</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>Expected RPAREN but got LPAREN</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Portfolio</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Product | Project</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Climate Change Mitigation</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Portfolio</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Product | Project</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>ePBN990097_1&amp;ePBN990103_1&amp;((ePBN114211_1&amp;ePBN990099_1&amp;ePBN990105_1)|((ePBN114211_1=0)&amp;ePBN990101_1))</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>FAILED</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>Unexpected token (</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>